<commit_message>
change predict income algorithm
</commit_message>
<xml_diff>
--- a/database/industries/biscuit/ghesalem/balancesheet/quarterly.xlsx
+++ b/database/industries/biscuit/ghesalem/balancesheet/quarterly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\ghaza\ghesalem\balancesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\biscuit\ghesalem\balancesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EF04E0-9CD4-488B-968A-0AC9AB2A3319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A05D4B-03E6-4C98-88D6-BDCA82F2D01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7176" yWindow="5148" windowWidth="13800" windowHeight="7092" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>دوره مالی</t>
   </si>
   <si>
-    <t>فصل دوم منتهی به 1399/06</t>
-  </si>
-  <si>
     <t>فصل سوم منتهی به 1399/09</t>
   </si>
   <si>
@@ -67,12 +64,12 @@
     <t>فصل سوم منتهی به 1401/09</t>
   </si>
   <si>
+    <t>فصل چهارم منتهی به 1401/12</t>
+  </si>
+  <si>
     <t>تاریخ انتشار</t>
   </si>
   <si>
-    <t>1399-08-28 (2)</t>
-  </si>
-  <si>
     <t>1399-10-27</t>
   </si>
   <si>
@@ -88,7 +85,7 @@
     <t>1400-10-29</t>
   </si>
   <si>
-    <t>1401-10-29 (6)</t>
+    <t>1402-02-30 (8)</t>
   </si>
   <si>
     <t>1401-04-28</t>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>1401-10-29</t>
+  </si>
+  <si>
+    <t>1402-02-30 (2)</t>
   </si>
   <si>
     <t>دارایی</t>
@@ -732,18 +732,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="31" customWidth="1"/>
-    <col min="11" max="13" width="29" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="31" customWidth="1"/>
+    <col min="10" max="12" width="29" customWidth="1"/>
+    <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -757,7 +758,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -773,7 +774,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -789,7 +790,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -803,7 +804,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -819,7 +820,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:13" ht="42" x14ac:dyDescent="0.65">
+    <row r="6" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -835,7 +836,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -849,7 +850,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -885,7 +886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -921,7 +922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -935,7 +936,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
@@ -951,43 +952,43 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15">
-        <v>158815</v>
+        <v>69417</v>
       </c>
       <c r="E12" s="15">
-        <v>69417</v>
+        <v>50630</v>
       </c>
       <c r="F12" s="15">
-        <v>50630</v>
+        <v>69044</v>
       </c>
       <c r="G12" s="15">
-        <v>69044</v>
+        <v>27220</v>
       </c>
       <c r="H12" s="15">
-        <v>27220</v>
+        <v>199788</v>
       </c>
       <c r="I12" s="15">
-        <v>199788</v>
+        <v>124711</v>
       </c>
       <c r="J12" s="15">
-        <v>124711</v>
+        <v>69166</v>
       </c>
       <c r="K12" s="15">
-        <v>69166</v>
+        <v>548992</v>
       </c>
       <c r="L12" s="15">
-        <v>548992</v>
+        <v>41389</v>
       </c>
       <c r="M12" s="15">
-        <v>41389</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+        <v>255126</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
@@ -1023,115 +1024,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15">
-        <v>588709</v>
+        <v>715852</v>
       </c>
       <c r="E14" s="15">
-        <v>715852</v>
+        <v>768470</v>
       </c>
       <c r="F14" s="15">
-        <v>768470</v>
+        <v>923574</v>
       </c>
       <c r="G14" s="15">
-        <v>923574</v>
+        <v>1322766</v>
       </c>
       <c r="H14" s="15">
-        <v>1322766</v>
+        <v>1417184</v>
       </c>
       <c r="I14" s="15">
-        <v>1417184</v>
+        <v>1298799</v>
       </c>
       <c r="J14" s="15">
-        <v>1298799</v>
+        <v>2115298</v>
       </c>
       <c r="K14" s="15">
-        <v>2115298</v>
+        <v>3035354</v>
       </c>
       <c r="L14" s="15">
-        <v>3035354</v>
+        <v>4658376</v>
       </c>
       <c r="M14" s="15">
-        <v>4658376</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+        <v>4133142</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11">
-        <v>435946</v>
+        <v>350186</v>
       </c>
       <c r="E15" s="11">
-        <v>350186</v>
+        <v>546798</v>
       </c>
       <c r="F15" s="11">
-        <v>546798</v>
+        <v>567628</v>
       </c>
       <c r="G15" s="11">
-        <v>567628</v>
+        <v>644099</v>
       </c>
       <c r="H15" s="11">
-        <v>644099</v>
+        <v>685158</v>
       </c>
       <c r="I15" s="11">
-        <v>685158</v>
+        <v>680684</v>
       </c>
       <c r="J15" s="11">
-        <v>680684</v>
+        <v>1389433</v>
       </c>
       <c r="K15" s="11">
-        <v>1389433</v>
+        <v>1206243</v>
       </c>
       <c r="L15" s="11">
-        <v>1206243</v>
+        <v>1373110</v>
       </c>
       <c r="M15" s="11">
-        <v>1373110</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+        <v>1509807</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15">
-        <v>17551</v>
+        <v>162688</v>
       </c>
       <c r="E16" s="15">
-        <v>162688</v>
+        <v>71616</v>
       </c>
       <c r="F16" s="15">
-        <v>71616</v>
+        <v>153655</v>
       </c>
       <c r="G16" s="15">
-        <v>153655</v>
+        <v>147025</v>
       </c>
       <c r="H16" s="15">
-        <v>147025</v>
+        <v>204791</v>
       </c>
       <c r="I16" s="15">
-        <v>204791</v>
+        <v>693571</v>
       </c>
       <c r="J16" s="15">
-        <v>693571</v>
+        <v>209930</v>
       </c>
       <c r="K16" s="15">
-        <v>209930</v>
+        <v>105015</v>
       </c>
       <c r="L16" s="15">
-        <v>105015</v>
+        <v>312655</v>
       </c>
       <c r="M16" s="15">
-        <v>312655</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+        <v>468936</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
@@ -1167,43 +1168,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17">
-        <v>1201021</v>
+        <v>1298143</v>
       </c>
       <c r="E18" s="17">
-        <v>1298143</v>
+        <v>1437514</v>
       </c>
       <c r="F18" s="17">
-        <v>1437514</v>
+        <v>1713901</v>
       </c>
       <c r="G18" s="17">
-        <v>1713901</v>
+        <v>2141110</v>
       </c>
       <c r="H18" s="17">
-        <v>2141110</v>
+        <v>2506921</v>
       </c>
       <c r="I18" s="17">
-        <v>2506921</v>
+        <v>2797765</v>
       </c>
       <c r="J18" s="17">
-        <v>2797765</v>
+        <v>3783827</v>
       </c>
       <c r="K18" s="17">
-        <v>3783827</v>
+        <v>4895604</v>
       </c>
       <c r="L18" s="17">
-        <v>4895604</v>
+        <v>6385530</v>
       </c>
       <c r="M18" s="17">
-        <v>6385530</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+        <v>6367011</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>34</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>35</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>36</v>
       </c>
@@ -1311,43 +1312,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15">
-        <v>4522658</v>
+        <v>4498746</v>
       </c>
       <c r="E22" s="15">
-        <v>4498746</v>
+        <v>4473707</v>
       </c>
       <c r="F22" s="15">
-        <v>4473707</v>
+        <v>4452375</v>
       </c>
       <c r="G22" s="15">
-        <v>4452375</v>
+        <v>4420163</v>
       </c>
       <c r="H22" s="15">
-        <v>4420163</v>
+        <v>4382650</v>
       </c>
       <c r="I22" s="15">
-        <v>4382650</v>
+        <v>4485773</v>
       </c>
       <c r="J22" s="15">
-        <v>4485773</v>
+        <v>4448774</v>
       </c>
       <c r="K22" s="15">
-        <v>4448774</v>
+        <v>4441313</v>
       </c>
       <c r="L22" s="15">
-        <v>4441313</v>
+        <v>4431833</v>
       </c>
       <c r="M22" s="15">
-        <v>4431833</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+        <v>4440095</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
         <v>38</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>39</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>41</v>
       </c>
@@ -1455,79 +1456,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17">
-        <v>4524029</v>
+        <v>4500117</v>
       </c>
       <c r="E26" s="17">
-        <v>4500117</v>
+        <v>4475078</v>
       </c>
       <c r="F26" s="17">
-        <v>4475078</v>
+        <v>4453746</v>
       </c>
       <c r="G26" s="17">
-        <v>4453746</v>
+        <v>4421534</v>
       </c>
       <c r="H26" s="17">
-        <v>4421534</v>
+        <v>4384021</v>
       </c>
       <c r="I26" s="17">
-        <v>4384021</v>
+        <v>4487144</v>
       </c>
       <c r="J26" s="17">
-        <v>4487144</v>
+        <v>4450145</v>
       </c>
       <c r="K26" s="17">
-        <v>4450145</v>
+        <v>4442684</v>
       </c>
       <c r="L26" s="17">
-        <v>4442684</v>
+        <v>4433204</v>
       </c>
       <c r="M26" s="17">
-        <v>4433204</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+        <v>4441466</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19">
-        <v>5725050</v>
+        <v>5798260</v>
       </c>
       <c r="E27" s="19">
-        <v>5798260</v>
+        <v>5912592</v>
       </c>
       <c r="F27" s="19">
-        <v>5912592</v>
+        <v>6167647</v>
       </c>
       <c r="G27" s="19">
-        <v>6167647</v>
+        <v>6562644</v>
       </c>
       <c r="H27" s="19">
-        <v>6562644</v>
+        <v>6890942</v>
       </c>
       <c r="I27" s="19">
-        <v>6890942</v>
+        <v>7284909</v>
       </c>
       <c r="J27" s="19">
-        <v>7284909</v>
+        <v>8233972</v>
       </c>
       <c r="K27" s="19">
-        <v>8233972</v>
+        <v>9338288</v>
       </c>
       <c r="L27" s="19">
-        <v>9338288</v>
+        <v>10818734</v>
       </c>
       <c r="M27" s="19">
-        <v>10818734</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <v>10808477</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>44</v>
       </c>
@@ -1543,43 +1544,43 @@
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15">
-        <v>312069</v>
+        <v>276627</v>
       </c>
       <c r="E29" s="15">
-        <v>276627</v>
+        <v>214295</v>
       </c>
       <c r="F29" s="15">
-        <v>214295</v>
+        <v>286806</v>
       </c>
       <c r="G29" s="15">
-        <v>286806</v>
+        <v>422459</v>
       </c>
       <c r="H29" s="15">
-        <v>422459</v>
+        <v>529206</v>
       </c>
       <c r="I29" s="15">
-        <v>529206</v>
+        <v>327294</v>
       </c>
       <c r="J29" s="15">
-        <v>327294</v>
+        <v>773044</v>
       </c>
       <c r="K29" s="15">
-        <v>773044</v>
+        <v>812952</v>
       </c>
       <c r="L29" s="15">
-        <v>812952</v>
+        <v>878852</v>
       </c>
       <c r="M29" s="15">
-        <v>878852</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+        <v>803973</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>46</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>47</v>
       </c>
@@ -1651,115 +1652,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11">
-        <v>81581</v>
+        <v>84420</v>
       </c>
       <c r="E32" s="11">
-        <v>84420</v>
+        <v>114998</v>
       </c>
       <c r="F32" s="11">
-        <v>114998</v>
+        <v>129858</v>
       </c>
       <c r="G32" s="11">
-        <v>129858</v>
+        <v>147534</v>
       </c>
       <c r="H32" s="11">
-        <v>147534</v>
+        <v>172675</v>
       </c>
       <c r="I32" s="11">
-        <v>172675</v>
+        <v>147625</v>
       </c>
       <c r="J32" s="11">
-        <v>147625</v>
+        <v>227816</v>
       </c>
       <c r="K32" s="11">
-        <v>227816</v>
+        <v>364392</v>
       </c>
       <c r="L32" s="11">
-        <v>364392</v>
+        <v>472171</v>
       </c>
       <c r="M32" s="11">
-        <v>472171</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+        <v>416996</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15">
-        <v>57752</v>
+        <v>57745</v>
       </c>
       <c r="E33" s="15">
-        <v>57745</v>
+        <v>5323</v>
       </c>
       <c r="F33" s="15">
-        <v>5323</v>
+        <v>5288</v>
       </c>
       <c r="G33" s="15">
-        <v>5288</v>
+        <v>229475</v>
       </c>
       <c r="H33" s="15">
-        <v>229475</v>
+        <v>133482</v>
       </c>
       <c r="I33" s="15">
-        <v>133482</v>
+        <v>8819</v>
       </c>
       <c r="J33" s="15">
-        <v>8819</v>
+        <v>8724</v>
       </c>
       <c r="K33" s="15">
-        <v>8724</v>
+        <v>455208</v>
       </c>
       <c r="L33" s="15">
-        <v>455208</v>
+        <v>263834</v>
       </c>
       <c r="M33" s="15">
-        <v>263834</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+        <v>11132</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11">
-        <v>37102</v>
+        <v>41498</v>
       </c>
       <c r="E34" s="11">
-        <v>41498</v>
+        <v>42755</v>
       </c>
       <c r="F34" s="11">
-        <v>42755</v>
+        <v>44051</v>
       </c>
       <c r="G34" s="11">
-        <v>44051</v>
+        <v>45386</v>
       </c>
       <c r="H34" s="11">
-        <v>45386</v>
+        <v>38575</v>
       </c>
       <c r="I34" s="11">
-        <v>38575</v>
+        <v>532549</v>
       </c>
       <c r="J34" s="11">
-        <v>532549</v>
+        <v>402903</v>
       </c>
       <c r="K34" s="11">
-        <v>402903</v>
+        <v>416876</v>
       </c>
       <c r="L34" s="11">
-        <v>416876</v>
+        <v>1078754</v>
       </c>
       <c r="M34" s="11">
-        <v>1078754</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+        <v>683417</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>51</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>52</v>
       </c>
@@ -1831,43 +1832,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17">
-        <v>488504</v>
+        <v>460290</v>
       </c>
       <c r="E37" s="17">
-        <v>460290</v>
+        <v>377371</v>
       </c>
       <c r="F37" s="17">
-        <v>377371</v>
+        <v>466003</v>
       </c>
       <c r="G37" s="17">
-        <v>466003</v>
+        <v>844854</v>
       </c>
       <c r="H37" s="17">
-        <v>844854</v>
+        <v>873938</v>
       </c>
       <c r="I37" s="17">
-        <v>873938</v>
+        <v>1016287</v>
       </c>
       <c r="J37" s="17">
-        <v>1016287</v>
+        <v>1412487</v>
       </c>
       <c r="K37" s="17">
-        <v>1412487</v>
+        <v>2049428</v>
       </c>
       <c r="L37" s="17">
-        <v>2049428</v>
+        <v>2693611</v>
       </c>
       <c r="M37" s="17">
-        <v>2693611</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+        <v>1915518</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
         <v>54</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="14" t="s">
         <v>55</v>
       </c>
@@ -1939,25 +1940,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11">
-        <v>49418</v>
+        <v>38575</v>
       </c>
       <c r="E40" s="11">
-        <v>38575</v>
+        <v>27403</v>
       </c>
       <c r="F40" s="11">
-        <v>27403</v>
+        <v>15892</v>
       </c>
       <c r="G40" s="11">
-        <v>15892</v>
+        <v>4032</v>
       </c>
       <c r="H40" s="11">
-        <v>4032</v>
+        <v>0</v>
       </c>
       <c r="I40" s="11">
         <v>0</v>
@@ -1975,115 +1976,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15">
-        <v>118853</v>
+        <v>129351</v>
       </c>
       <c r="E41" s="15">
-        <v>129351</v>
+        <v>130856</v>
       </c>
       <c r="F41" s="15">
-        <v>130856</v>
+        <v>147507</v>
       </c>
       <c r="G41" s="15">
-        <v>147507</v>
+        <v>170541</v>
       </c>
       <c r="H41" s="15">
-        <v>170541</v>
+        <v>221949</v>
       </c>
       <c r="I41" s="15">
-        <v>221949</v>
+        <v>250921</v>
       </c>
       <c r="J41" s="15">
-        <v>250921</v>
+        <v>291630</v>
       </c>
       <c r="K41" s="15">
-        <v>291630</v>
+        <v>332557</v>
       </c>
       <c r="L41" s="15">
-        <v>332557</v>
+        <v>365179</v>
       </c>
       <c r="M41" s="15">
-        <v>365179</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+        <v>406132</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19">
-        <v>168271</v>
+        <v>167926</v>
       </c>
       <c r="E42" s="19">
-        <v>167926</v>
+        <v>158259</v>
       </c>
       <c r="F42" s="19">
-        <v>158259</v>
+        <v>163399</v>
       </c>
       <c r="G42" s="19">
-        <v>163399</v>
+        <v>174573</v>
       </c>
       <c r="H42" s="19">
-        <v>174573</v>
+        <v>221949</v>
       </c>
       <c r="I42" s="19">
-        <v>221949</v>
+        <v>250921</v>
       </c>
       <c r="J42" s="19">
-        <v>250921</v>
+        <v>291630</v>
       </c>
       <c r="K42" s="19">
-        <v>291630</v>
+        <v>332557</v>
       </c>
       <c r="L42" s="19">
-        <v>332557</v>
+        <v>365179</v>
       </c>
       <c r="M42" s="19">
-        <v>365179</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+        <v>406132</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17">
-        <v>656775</v>
+        <v>628216</v>
       </c>
       <c r="E43" s="17">
-        <v>628216</v>
+        <v>535630</v>
       </c>
       <c r="F43" s="17">
-        <v>535630</v>
+        <v>629402</v>
       </c>
       <c r="G43" s="17">
-        <v>629402</v>
+        <v>1019427</v>
       </c>
       <c r="H43" s="17">
-        <v>1019427</v>
+        <v>1095887</v>
       </c>
       <c r="I43" s="17">
-        <v>1095887</v>
+        <v>1267208</v>
       </c>
       <c r="J43" s="17">
-        <v>1267208</v>
+        <v>1704117</v>
       </c>
       <c r="K43" s="17">
-        <v>1704117</v>
+        <v>2381985</v>
       </c>
       <c r="L43" s="17">
-        <v>2381985</v>
+        <v>3058790</v>
       </c>
       <c r="M43" s="17">
-        <v>3058790</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+        <v>2321650</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="12" t="s">
         <v>60</v>
       </c>
@@ -2099,7 +2100,7 @@
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>61</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>4484000</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" s="14" t="s">
         <v>63</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
         <v>65</v>
       </c>
@@ -2279,43 +2280,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="11">
-        <v>38572</v>
+        <v>43660</v>
       </c>
       <c r="E50" s="11">
-        <v>43660</v>
+        <v>54006</v>
       </c>
       <c r="F50" s="11">
-        <v>54006</v>
+        <v>62070</v>
       </c>
       <c r="G50" s="11">
-        <v>62070</v>
+        <v>73529</v>
       </c>
       <c r="H50" s="11">
-        <v>73529</v>
+        <v>86121</v>
       </c>
       <c r="I50" s="11">
-        <v>86121</v>
+        <v>97253</v>
       </c>
       <c r="J50" s="11">
-        <v>97253</v>
+        <v>122861</v>
       </c>
       <c r="K50" s="11">
-        <v>122861</v>
+        <v>166603</v>
       </c>
       <c r="L50" s="11">
-        <v>166603</v>
+        <v>206785</v>
       </c>
       <c r="M50" s="11">
-        <v>206785</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+        <v>243129</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
         <v>67</v>
       </c>
@@ -2351,7 +2352,7 @@
         <v>12895</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>68</v>
       </c>
@@ -2387,43 +2388,43 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15">
-        <v>18548</v>
+        <v>18386</v>
       </c>
       <c r="E53" s="15">
-        <v>18386</v>
+        <v>18350</v>
       </c>
       <c r="F53" s="15">
-        <v>18350</v>
+        <v>18187</v>
       </c>
       <c r="G53" s="15">
-        <v>18187</v>
+        <v>18025</v>
       </c>
       <c r="H53" s="15">
-        <v>18025</v>
+        <v>17862</v>
       </c>
       <c r="I53" s="15">
-        <v>17862</v>
+        <v>17827</v>
       </c>
       <c r="J53" s="15">
-        <v>17827</v>
+        <v>17696</v>
       </c>
       <c r="K53" s="15">
-        <v>17696</v>
+        <v>17502</v>
       </c>
       <c r="L53" s="15">
-        <v>17502</v>
+        <v>17042</v>
       </c>
       <c r="M53" s="15">
-        <v>17042</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+        <v>17304</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>70</v>
       </c>
@@ -2459,7 +2460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="14" t="s">
         <v>71</v>
       </c>
@@ -2495,115 +2496,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11">
-        <v>514260</v>
+        <v>611103</v>
       </c>
       <c r="E56" s="11">
-        <v>611103</v>
+        <v>807711</v>
       </c>
       <c r="F56" s="11">
-        <v>807711</v>
+        <v>961093</v>
       </c>
       <c r="G56" s="11">
-        <v>961093</v>
+        <v>954768</v>
       </c>
       <c r="H56" s="11">
-        <v>954768</v>
+        <v>1194177</v>
       </c>
       <c r="I56" s="11">
-        <v>1194177</v>
+        <v>1405726</v>
       </c>
       <c r="J56" s="11">
-        <v>1405726</v>
+        <v>1892403</v>
       </c>
       <c r="K56" s="11">
-        <v>1892403</v>
+        <v>2275303</v>
       </c>
       <c r="L56" s="11">
-        <v>2275303</v>
+        <v>3039222</v>
       </c>
       <c r="M56" s="11">
-        <v>3039222</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+        <v>3729499</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17">
-        <v>5068275</v>
+        <v>5170044</v>
       </c>
       <c r="E57" s="17">
-        <v>5170044</v>
+        <v>5376962</v>
       </c>
       <c r="F57" s="17">
-        <v>5376962</v>
+        <v>5538245</v>
       </c>
       <c r="G57" s="17">
-        <v>5538245</v>
+        <v>5543217</v>
       </c>
       <c r="H57" s="17">
-        <v>5543217</v>
+        <v>5795055</v>
       </c>
       <c r="I57" s="17">
-        <v>5795055</v>
+        <v>6017701</v>
       </c>
       <c r="J57" s="17">
-        <v>6017701</v>
+        <v>6529855</v>
       </c>
       <c r="K57" s="17">
-        <v>6529855</v>
+        <v>6956303</v>
       </c>
       <c r="L57" s="17">
-        <v>6956303</v>
+        <v>7759944</v>
       </c>
       <c r="M57" s="17">
-        <v>7759944</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+        <v>8486827</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19">
-        <v>5725050</v>
+        <v>5798260</v>
       </c>
       <c r="E58" s="19">
-        <v>5798260</v>
+        <v>5912592</v>
       </c>
       <c r="F58" s="19">
-        <v>5912592</v>
+        <v>6167647</v>
       </c>
       <c r="G58" s="19">
-        <v>6167647</v>
+        <v>6562644</v>
       </c>
       <c r="H58" s="19">
-        <v>6562644</v>
+        <v>6890942</v>
       </c>
       <c r="I58" s="19">
-        <v>6890942</v>
+        <v>7284909</v>
       </c>
       <c r="J58" s="19">
-        <v>7284909</v>
+        <v>8233972</v>
       </c>
       <c r="K58" s="19">
-        <v>8233972</v>
+        <v>9338288</v>
       </c>
       <c r="L58" s="19">
-        <v>9338288</v>
+        <v>10818734</v>
       </c>
       <c r="M58" s="19">
-        <v>10818734</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+        <v>10808477</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>

</xml_diff>